<commit_message>
i hate this model
</commit_message>
<xml_diff>
--- a/GOA/Model runs/GOA_18.5.1/Data/2018_SAFE_pollock_estimates.xlsx
+++ b/GOA/Model runs/GOA_18.5.1/Data/2018_SAFE_pollock_estimates.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="885" yWindow="1455" windowWidth="24645" windowHeight="13380" activeTab="2"/>
+    <workbookView xWindow="885" yWindow="1455" windowWidth="24645" windowHeight="13380" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Biomass" sheetId="1" r:id="rId1"/>
     <sheet name="SSB" sheetId="2" r:id="rId2"/>
     <sheet name="R" sheetId="3" r:id="rId3"/>
+    <sheet name="Catch" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,12 +33,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>2018_Pollock</t>
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>1977_2018_safe</t>
+  </si>
+  <si>
+    <t>1977_2018_non_equilibrium_safe</t>
+  </si>
+  <si>
+    <t>2018_Pollock_non_equilibrium</t>
+  </si>
+  <si>
+    <t>Total catch</t>
   </si>
 </sst>
 </file>
@@ -406,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -417,404 +430,809 @@
     <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1970</v>
       </c>
       <c r="B2">
         <v>0.53393299999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>0.52455499999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1971</v>
       </c>
       <c r="B3">
         <v>0.493203</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>0.490923</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1972</v>
       </c>
       <c r="B4">
         <v>0.45936199999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>0.45777699999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1973</v>
       </c>
       <c r="B5">
         <v>0.50888199999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>0.50788699999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1974</v>
       </c>
       <c r="B6">
         <v>0.57046300000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>0.56975600000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1975</v>
       </c>
       <c r="B7">
         <v>0.99719000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>0.99659900000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1976</v>
       </c>
       <c r="B8">
         <v>0.89083100000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>0.89033399999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1977</v>
       </c>
       <c r="B9">
         <v>0.74619599999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>3.31324</v>
+      </c>
+      <c r="D9">
+        <v>1.65052</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.74582700000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1978</v>
       </c>
       <c r="B10">
         <v>0.96472400000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2.9862500000000001</v>
+      </c>
+      <c r="D10">
+        <v>1.95147</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.96443500000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1979</v>
       </c>
       <c r="B11">
         <v>1.3463499999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2.74214</v>
+      </c>
+      <c r="D11">
+        <v>1.7078100000000001</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1.34606</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1980</v>
       </c>
       <c r="B12">
         <v>1.8120499999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>3.08771</v>
+      </c>
+      <c r="D12">
+        <v>2.2238199999999999</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.8117399999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1981</v>
       </c>
       <c r="B13">
         <v>2.83155</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>3.9476800000000001</v>
+      </c>
+      <c r="D13">
+        <v>3.1188600000000002</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2.8311700000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1982</v>
       </c>
       <c r="B14">
         <v>2.9555899999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>3.87696</v>
+      </c>
+      <c r="D14">
+        <v>3.1796799999999998</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2.9552200000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1983</v>
       </c>
       <c r="B15">
         <v>2.69068</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>3.4404300000000001</v>
+      </c>
+      <c r="D15">
+        <v>2.8569100000000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2.69035</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1984</v>
       </c>
       <c r="B16">
         <v>2.3905400000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>2.9929299999999999</v>
+      </c>
+      <c r="D16">
+        <v>2.51858</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.39025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1985</v>
       </c>
       <c r="B17">
         <v>1.92954</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>2.4245899999999998</v>
+      </c>
+      <c r="D17">
+        <v>2.0453199999999998</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.92927</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1986</v>
       </c>
       <c r="B18">
         <v>1.62215</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2.07802</v>
+      </c>
+      <c r="D18">
+        <v>1.74638</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.6219300000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1987</v>
       </c>
       <c r="B19">
         <v>1.96593</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2.44198</v>
+      </c>
+      <c r="D19">
+        <v>2.12988</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.9657100000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1988</v>
       </c>
       <c r="B20">
         <v>1.8635699999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>2.2970100000000002</v>
+      </c>
+      <c r="D20">
+        <v>2.02122</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.86337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1989</v>
       </c>
       <c r="B21">
         <v>1.6474200000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>2.0184000000000002</v>
+      </c>
+      <c r="D21">
+        <v>1.7907299999999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.6472500000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1990</v>
       </c>
       <c r="B22">
         <v>1.5252399999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>1.86351</v>
+      </c>
+      <c r="D22">
+        <v>1.6606799999999999</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.5250900000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1991</v>
       </c>
       <c r="B23">
         <v>1.8397600000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2.2083900000000001</v>
+      </c>
+      <c r="D23">
+        <v>2.0004599999999999</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.83961</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1992</v>
       </c>
       <c r="B24">
         <v>1.9216200000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>2.3071000000000002</v>
+      </c>
+      <c r="D24">
+        <v>2.0958399999999999</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1.9214599999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1993</v>
       </c>
       <c r="B25">
         <v>1.8085199999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>2.1761699999999999</v>
+      </c>
+      <c r="D25">
+        <v>1.9785299999999999</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1.8083800000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1994</v>
       </c>
       <c r="B26">
         <v>1.53277</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>1.8511599999999999</v>
+      </c>
+      <c r="D26">
+        <v>1.6816500000000001</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1.5326500000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1995</v>
       </c>
       <c r="B27">
         <v>1.2519100000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1.5181800000000001</v>
+      </c>
+      <c r="D27">
+        <v>1.37754</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1.2518100000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1996</v>
       </c>
       <c r="B28">
         <v>1.05192</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>1.27725</v>
+      </c>
+      <c r="D28">
+        <v>1.1590499999999999</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1.0518400000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1997</v>
       </c>
       <c r="B29">
         <v>1.0734900000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1.28145</v>
+      </c>
+      <c r="D29">
+        <v>1.1727399999999999</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.07342</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1998</v>
       </c>
       <c r="B30">
         <v>1.0323800000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>1.23214</v>
+      </c>
+      <c r="D30">
+        <v>1.1281000000000001</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1.0323199999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1999</v>
       </c>
       <c r="B31">
         <v>0.76931700000000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>0.93577100000000002</v>
+      </c>
+      <c r="D31">
+        <v>0.84926199999999996</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.76926300000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2000</v>
       </c>
       <c r="B32">
         <v>0.68083899999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>0.84011000000000002</v>
+      </c>
+      <c r="D32">
+        <v>0.75752600000000003</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.68078899999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2001</v>
       </c>
       <c r="B33">
         <v>0.65116600000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>0.80885799999999997</v>
+      </c>
+      <c r="D33">
+        <v>0.72726999999999997</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.651119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2002</v>
       </c>
       <c r="B34">
         <v>0.84367300000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>1.0337099999999999</v>
+      </c>
+      <c r="D34">
+        <v>0.93492399999999998</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.84361699999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2003</v>
       </c>
       <c r="B35">
         <v>1.0645199999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1.28982</v>
+      </c>
+      <c r="D35">
+        <v>1.1721200000000001</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1.06446</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2004</v>
       </c>
       <c r="B36">
         <v>0.89120699999999997</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>1.08609</v>
+      </c>
+      <c r="D36">
+        <v>0.98457099999999997</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.89115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2005</v>
       </c>
       <c r="B37">
         <v>0.74539100000000003</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>0.91665399999999997</v>
+      </c>
+      <c r="D37">
+        <v>0.82760800000000001</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.74534100000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2006</v>
       </c>
       <c r="B38">
         <v>0.63585199999999997</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>0.79650600000000005</v>
+      </c>
+      <c r="D38">
+        <v>0.71310300000000004</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.63580599999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2007</v>
       </c>
       <c r="B39">
         <v>0.59550800000000004</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>0.75423899999999999</v>
+      </c>
+      <c r="D39">
+        <v>0.672099</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.59546200000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2008</v>
       </c>
       <c r="B40">
         <v>0.82730300000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>1.0289900000000001</v>
+      </c>
+      <c r="D40">
+        <v>0.92486299999999999</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.82724500000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2009</v>
       </c>
       <c r="B41">
         <v>1.1698</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>1.43675</v>
+      </c>
+      <c r="D41">
+        <v>1.2994399999999999</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1.1697299999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2010</v>
       </c>
       <c r="B42">
         <v>1.38096</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>1.6791199999999999</v>
+      </c>
+      <c r="D42">
+        <v>1.5267900000000001</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1.3808800000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2011</v>
       </c>
       <c r="B43">
         <v>1.3168299999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>1.60195</v>
+      </c>
+      <c r="D43">
+        <v>1.4571700000000001</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1.3167599999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2012</v>
       </c>
       <c r="B44">
         <v>1.2238100000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>1.4961599999999999</v>
+      </c>
+      <c r="D44">
+        <v>1.35873</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1.22374</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2013</v>
       </c>
       <c r="B45">
         <v>1.25563</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>1.5314099999999999</v>
+      </c>
+      <c r="D45">
+        <v>1.39341</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1.25556</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2014</v>
       </c>
       <c r="B46">
         <v>0.99460700000000002</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>1.21993</v>
+      </c>
+      <c r="D46">
+        <v>1.10795</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.99454500000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2015</v>
       </c>
       <c r="B47">
         <v>2.3446899999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>2.7804700000000002</v>
+      </c>
+      <c r="D47">
+        <v>2.56576</v>
+      </c>
+      <c r="E47" s="1">
+        <v>2.34456</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2016</v>
       </c>
       <c r="B48">
         <v>2.3071000000000002</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>2.7487599999999999</v>
+      </c>
+      <c r="D48">
+        <v>2.5323600000000002</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2.3069799999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2017</v>
       </c>
       <c r="B49">
         <v>1.6718900000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>2.0277400000000001</v>
+      </c>
+      <c r="D49">
+        <v>1.8535200000000001</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1.6717900000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2018</v>
       </c>
       <c r="B50">
         <v>1.1862900000000001</v>
+      </c>
+      <c r="C50">
+        <v>1.4798</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1.18621</v>
       </c>
     </row>
   </sheetData>
@@ -824,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:AZ2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -835,404 +1253,809 @@
     <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1970</v>
       </c>
       <c r="B2" s="1">
         <v>0.125226</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>0.12396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1971</v>
       </c>
       <c r="B3" s="1">
         <v>0.119645</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>0.118114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1972</v>
       </c>
       <c r="B4" s="1">
         <v>0.110057</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>0.10879999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1973</v>
       </c>
       <c r="B5" s="1">
         <v>9.2260700000000001E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>9.1529399999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1974</v>
       </c>
       <c r="B6" s="1">
         <v>8.2707299999999997E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>8.2347900000000002E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1975</v>
       </c>
       <c r="B7" s="1">
         <v>8.5445900000000005E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>8.5189699999999993E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1976</v>
       </c>
       <c r="B8" s="1">
         <v>0.121253</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>0.121056</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1977</v>
       </c>
       <c r="B9" s="1">
         <v>0.132461</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>0.77302400000000004</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.36773899999999998</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.13231899999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1978</v>
       </c>
       <c r="B10" s="1">
         <v>0.117405</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>0.72026199999999996</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.34534900000000002</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.117317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1979</v>
       </c>
       <c r="B11" s="1">
         <v>0.124393</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>0.66498800000000002</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.33874900000000002</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.124323</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1980</v>
       </c>
       <c r="B12" s="1">
         <v>0.17233299999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>0.60901099999999997</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.33679300000000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.17227000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1981</v>
       </c>
       <c r="B13" s="1">
         <v>0.188641</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>0.47622999999999999</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.29456399999999999</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.18859300000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1982</v>
       </c>
       <c r="B14" s="1">
         <v>0.32290200000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>0.58344799999999997</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.40280100000000002</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.32284099999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1983</v>
       </c>
       <c r="B15" s="1">
         <v>0.45052999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>0.70479599999999998</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.52951800000000004</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.45045600000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1984</v>
       </c>
       <c r="B16" s="1">
         <v>0.50071900000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>0.71067100000000005</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.55579400000000001</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.50063899999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1985</v>
       </c>
       <c r="B17" s="1">
         <v>0.45560899999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>0.64593400000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.505247</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.45552900000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1986</v>
       </c>
       <c r="B18" s="1">
         <v>0.41200999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>0.56135800000000002</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.44378600000000001</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.41193299999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1987</v>
       </c>
       <c r="B19" s="1">
         <v>0.38422899999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>0.51843600000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.4153</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.384158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1988</v>
       </c>
       <c r="B20" s="1">
         <v>0.39489999999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>0.52042999999999995</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.42708600000000002</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.39483499999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1989</v>
       </c>
       <c r="B21" s="1">
         <v>0.408026</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>0.519679</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.44279099999999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.40796900000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1990</v>
       </c>
       <c r="B22" s="1">
         <v>0.41778700000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <v>0.52742599999999995</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.45619199999999999</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.41773399999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1991</v>
       </c>
       <c r="B23" s="1">
         <v>0.41153899999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>0.51783000000000001</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.45158399999999999</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.41149000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1992</v>
       </c>
       <c r="B24" s="1">
         <v>0.37707000000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <v>0.46946900000000003</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.41586299999999998</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.37702999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1993</v>
       </c>
       <c r="B25" s="1">
         <v>0.41082800000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <v>0.50795199999999996</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.45386399999999999</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.41078700000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1994</v>
       </c>
       <c r="B26" s="1">
         <v>0.48249900000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <v>0.59453500000000004</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.53403299999999998</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.48245500000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1995</v>
       </c>
       <c r="B27" s="1">
         <v>0.40185300000000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <v>0.497728</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.44643899999999997</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.40181600000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1996</v>
       </c>
       <c r="B28" s="1">
         <v>0.37068699999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <v>0.45866099999999999</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.41206900000000002</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.37065300000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1997</v>
       </c>
       <c r="B29" s="1">
         <v>0.32724199999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <v>0.40606500000000001</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.36463499999999999</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.327212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1998</v>
       </c>
       <c r="B30" s="1">
         <v>0.25525399999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <v>0.32067499999999999</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.286495</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.25522899999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1999</v>
       </c>
       <c r="B31" s="1">
         <v>0.23660100000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <v>0.29968099999999998</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.266849</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.23657800000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2000</v>
       </c>
       <c r="B32" s="1">
         <v>0.22375900000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <v>0.28500199999999998</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.25317499999999998</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.22373799999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2001</v>
       </c>
       <c r="B33" s="1">
         <v>0.209368</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <v>0.26945599999999997</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.238264</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.20934800000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2002</v>
       </c>
       <c r="B34" s="1">
         <v>0.17399400000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <v>0.22713900000000001</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.199604</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.17397699999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2003</v>
       </c>
       <c r="B35" s="1">
         <v>0.162934</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <v>0.21099799999999999</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.186089</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.16291900000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2004</v>
       </c>
       <c r="B36" s="1">
         <v>0.184119</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <v>0.23219100000000001</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.207237</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.18410499999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2005</v>
       </c>
       <c r="B37" s="1">
         <v>0.22253000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
+        <v>0.28173300000000001</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.25092500000000001</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.22251199999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2006</v>
       </c>
       <c r="B38" s="1">
         <v>0.24093800000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="1">
+        <v>0.30745800000000001</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.27280900000000002</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0.24091899999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2007</v>
       </c>
       <c r="B39" s="1">
         <v>0.21387200000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="1">
+        <v>0.27721299999999999</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.24426300000000001</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.21385399999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2008</v>
       </c>
       <c r="B40" s="1">
         <v>0.21205199999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="1">
+        <v>0.27646199999999999</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.243035</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0.212034</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2009</v>
       </c>
       <c r="B41" s="1">
         <v>0.212233</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="1">
+        <v>0.27496199999999998</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.242507</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0.21221499999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2010</v>
       </c>
       <c r="B42" s="1">
         <v>0.28963800000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="1">
+        <v>0.36577900000000002</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.32657700000000001</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0.28961700000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2011</v>
       </c>
       <c r="B43" s="1">
         <v>0.33972799999999997</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="1">
+        <v>0.423537</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.38057400000000002</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0.33970499999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2012</v>
       </c>
       <c r="B44" s="1">
         <v>0.35992299999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="1">
+        <v>0.448127</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.40314800000000001</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.35989900000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2013</v>
       </c>
       <c r="B45" s="1">
         <v>0.38547300000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" s="1">
+        <v>0.48398000000000002</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.43406299999999998</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.38544699999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2014</v>
       </c>
       <c r="B46" s="1">
         <v>0.29852699999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" s="1">
+        <v>0.37729200000000002</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.33768799999999999</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.29850599999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2015</v>
       </c>
       <c r="B47" s="1">
         <v>0.26089099999999998</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="1">
+        <v>0.33614899999999998</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.29857600000000001</v>
+      </c>
+      <c r="E47" s="1">
+        <v>0.26086999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2016</v>
       </c>
       <c r="B48" s="1">
         <v>0.28238200000000002</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="1">
+        <v>0.352489</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.317797</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.282362</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2017</v>
       </c>
       <c r="B49" s="1">
         <v>0.35184799999999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="1">
+        <v>0.43958199999999997</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.39633400000000002</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.351823</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2018</v>
       </c>
       <c r="B50" s="1">
         <v>0.325544</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.41470200000000002</v>
+      </c>
+      <c r="E50" s="1">
+        <v>0.325519</v>
       </c>
     </row>
   </sheetData>
@@ -1242,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1253,404 +2076,1377 @@
     <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1970</v>
       </c>
       <c r="B2" s="1">
         <v>1.2546299999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>1.2563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1971</v>
       </c>
       <c r="B3" s="1">
         <v>3.17794</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>3.1789999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1972</v>
       </c>
       <c r="B4" s="1">
         <v>3.6379600000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>3.6387999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1973</v>
       </c>
       <c r="B5" s="1">
         <v>10.545500000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>10.545</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1974</v>
       </c>
       <c r="B6" s="1">
         <v>2.1892</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>2.1890999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1975</v>
       </c>
       <c r="B7" s="1">
         <v>2.2095699999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>2.2092999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1976</v>
       </c>
       <c r="B8" s="1">
         <v>8.6606799999999993</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>8.6595999999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1977</v>
       </c>
       <c r="B9" s="2">
         <v>11.7095</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>7.78</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.0407000000000002</v>
+      </c>
+      <c r="E9" s="1">
+        <v>11.708</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1978</v>
       </c>
       <c r="B10" s="2">
         <v>14.321099999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D10" s="1">
+        <v>16.661999999999999</v>
+      </c>
+      <c r="E10" s="1">
+        <v>14.319000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1979</v>
       </c>
       <c r="B11" s="2">
         <v>25.424800000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>27.4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>24.949000000000002</v>
+      </c>
+      <c r="E11" s="1">
+        <v>25.422000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1980</v>
       </c>
       <c r="B12" s="2">
         <v>12.958600000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="D12" s="1">
+        <v>12.848000000000001</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12.957000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1981</v>
       </c>
       <c r="B13" s="2">
         <v>7.2314800000000004</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="D13" s="1">
+        <v>7.1775000000000002</v>
+      </c>
+      <c r="E13" s="1">
+        <v>7.2308000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1982</v>
       </c>
       <c r="B14" s="2">
         <v>7.2290400000000004</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>7.67</v>
+      </c>
+      <c r="D14" s="1">
+        <v>7.2884000000000002</v>
+      </c>
+      <c r="E14" s="1">
+        <v>7.2286000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1983</v>
       </c>
       <c r="B15" s="2">
         <v>4.96774</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>5.25</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.1679000000000004</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4.9671000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1984</v>
       </c>
       <c r="B16" s="2">
         <v>5.9334499999999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>7.23</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.6363000000000003</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5.9333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1985</v>
       </c>
       <c r="B17" s="2">
         <v>14.760199999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1">
+        <v>16.128</v>
+      </c>
+      <c r="E17" s="1">
+        <v>14.759</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1986</v>
       </c>
       <c r="B18" s="2">
         <v>4.3154000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>4.82</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4.6139000000000001</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4.3151000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1987</v>
       </c>
       <c r="B19" s="2">
         <v>1.7894699999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>2.09</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.9686999999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.7892999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1988</v>
       </c>
       <c r="B20" s="2">
         <v>4.9982499999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="D20" s="1">
+        <v>5.3654999999999999</v>
+      </c>
+      <c r="E20" s="1">
+        <v>4.9978999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1989</v>
       </c>
       <c r="B21" s="2">
         <v>11.468500000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>13.2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>12.343999999999999</v>
+      </c>
+      <c r="E21" s="1">
+        <v>11.467000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1990</v>
       </c>
       <c r="B22" s="2">
         <v>8.4519300000000008</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="D22" s="1">
+        <v>9.1829999999999998</v>
+      </c>
+      <c r="E22" s="1">
+        <v>8.4513999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1991</v>
       </c>
       <c r="B23" s="2">
         <v>3.2506300000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>3.81</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3.5268000000000002</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3.2504</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1992</v>
       </c>
       <c r="B24" s="2">
         <v>2.3623500000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <v>2.64</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2.5066000000000002</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2.3622000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1993</v>
       </c>
       <c r="B25" s="2">
         <v>1.66597</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <v>1.85</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1.7647999999999999</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1.6658999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1994</v>
       </c>
       <c r="B26" s="2">
         <v>1.7010799999999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <v>1.92</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.8181</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1.7010000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1995</v>
       </c>
       <c r="B27" s="2">
         <v>6.7394699999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <v>7.55</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7.1276000000000002</v>
+      </c>
+      <c r="E27" s="1">
+        <v>6.7392000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1996</v>
       </c>
       <c r="B28" s="2">
         <v>3.1549</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <v>3.61</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3.3803000000000001</v>
+      </c>
+      <c r="E28" s="1">
+        <v>3.1547000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1997</v>
       </c>
       <c r="B29" s="2">
         <v>1.45472</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <v>1.72</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1.5884</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.4545999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1998</v>
       </c>
       <c r="B30" s="2">
         <v>1.4021399999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <v>1.66</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1.5287999999999999</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1.4019999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1999</v>
       </c>
       <c r="B31" s="2">
         <v>1.7577799999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1.9104000000000001</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1.7577</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2000</v>
       </c>
       <c r="B32" s="2">
         <v>6.62507</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="D32" s="1">
+        <v>7.1604999999999999</v>
+      </c>
+      <c r="E32" s="1">
+        <v>6.6246999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2001</v>
       </c>
       <c r="B33" s="2">
         <v>7.11416</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <v>8.32</v>
+      </c>
+      <c r="D33" s="1">
+        <v>7.6855000000000002</v>
+      </c>
+      <c r="E33" s="1">
+        <v>7.1138000000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2002</v>
       </c>
       <c r="B34" s="2">
         <v>1.0038400000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <v>1.18</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.0931</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.0038</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2003</v>
       </c>
       <c r="B35" s="2">
         <v>0.77695999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.84260000000000002</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.77690000000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2004</v>
       </c>
       <c r="B36" s="2">
         <v>0.73172000000000004</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.73160000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2005</v>
       </c>
       <c r="B37" s="2">
         <v>1.8793200000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
+        <v>2.19</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2.0377000000000001</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1.8792</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2006</v>
       </c>
       <c r="B38" s="2">
         <v>6.02555</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>6.5479000000000003</v>
+      </c>
+      <c r="E38" s="1">
+        <v>6.0251999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2007</v>
       </c>
       <c r="B39" s="2">
         <v>5.6892300000000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="1">
+        <v>6.76</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6.2144000000000004</v>
+      </c>
+      <c r="E39" s="1">
+        <v>5.6889000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2008</v>
       </c>
       <c r="B40" s="2">
         <v>7.0248699999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="1">
+        <v>8.26</v>
+      </c>
+      <c r="D40" s="1">
+        <v>7.6417999999999999</v>
+      </c>
+      <c r="E40" s="1">
+        <v>7.0244999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2009</v>
       </c>
       <c r="B41" s="2">
         <v>3.1086399999999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="1">
+        <v>3.62</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3.3759000000000001</v>
+      </c>
+      <c r="E41" s="1">
+        <v>3.1084999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2010</v>
       </c>
       <c r="B42" s="2">
         <v>1.2157899999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="1">
+        <v>1.42</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1.3282</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1.2157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2011</v>
       </c>
       <c r="B43" s="2">
         <v>5.2729600000000003</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="1">
+        <v>6.08</v>
+      </c>
+      <c r="D43" s="1">
+        <v>5.6866000000000003</v>
+      </c>
+      <c r="E43" s="1">
+        <v>5.2727000000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2012</v>
       </c>
       <c r="B44" s="2">
         <v>0.85650000000000004</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="1">
+        <v>1.01</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.94630000000000003</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.85640000000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2013</v>
       </c>
       <c r="B45" s="2">
         <v>37.178699999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" s="1">
+        <v>43</v>
+      </c>
+      <c r="D45" s="1">
+        <v>40.155999999999999</v>
+      </c>
+      <c r="E45" s="1">
+        <v>37.177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2014</v>
       </c>
       <c r="B46" s="2">
         <v>2.0390799999999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" s="1">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="D46" s="1">
+        <v>2.2545999999999999</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2.0390000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2015</v>
       </c>
       <c r="B47" s="2">
         <v>3.7879999999999997E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="D47" s="1">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="E47" s="1">
+        <v>3.78E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2016</v>
       </c>
       <c r="B48" s="2">
         <v>5.9500000000000004E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="1">
+        <v>7.1637799999999998E-3</v>
+      </c>
+      <c r="D48" s="1">
+        <v>6.6E-3</v>
+      </c>
+      <c r="E48" s="1">
+        <v>5.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2017</v>
       </c>
       <c r="B49" s="2">
         <v>2.1241599999999998</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="1">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="D49" s="1">
+        <v>2.3475000000000001</v>
+      </c>
+      <c r="E49" s="1">
+        <v>2.1240000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2018</v>
       </c>
       <c r="B50" s="2">
         <v>5.4148800000000001</v>
+      </c>
+      <c r="C50" s="1">
+        <v>6.53</v>
+      </c>
+      <c r="D50" s="1">
+        <v>6.0522999999999998</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5.4146999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1970</v>
+      </c>
+      <c r="B2">
+        <v>9379</v>
+      </c>
+      <c r="C2">
+        <v>9379.49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1971</v>
+      </c>
+      <c r="B3">
+        <v>9460</v>
+      </c>
+      <c r="C3">
+        <v>9460.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1972</v>
+      </c>
+      <c r="B4">
+        <v>38131</v>
+      </c>
+      <c r="C4">
+        <v>38141.599999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1973</v>
+      </c>
+      <c r="B5">
+        <v>44993</v>
+      </c>
+      <c r="C5">
+        <v>45007.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1974</v>
+      </c>
+      <c r="B6">
+        <v>61905</v>
+      </c>
+      <c r="C6">
+        <v>61925</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1975</v>
+      </c>
+      <c r="B7">
+        <v>59504</v>
+      </c>
+      <c r="C7">
+        <v>59506.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1976</v>
+      </c>
+      <c r="B8">
+        <v>86731</v>
+      </c>
+      <c r="C8">
+        <v>86695.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B9">
+        <v>118092</v>
+      </c>
+      <c r="C9">
+        <v>118080</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1978</v>
+      </c>
+      <c r="B10">
+        <v>95408</v>
+      </c>
+      <c r="C10">
+        <v>95419.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1979</v>
+      </c>
+      <c r="B11">
+        <v>106161</v>
+      </c>
+      <c r="C11">
+        <v>106080</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1980</v>
+      </c>
+      <c r="B12">
+        <v>115158</v>
+      </c>
+      <c r="C12">
+        <v>115215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1981</v>
+      </c>
+      <c r="B13">
+        <v>147818</v>
+      </c>
+      <c r="C13">
+        <v>147873</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1982</v>
+      </c>
+      <c r="B14">
+        <v>169045</v>
+      </c>
+      <c r="C14">
+        <v>168981</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1983</v>
+      </c>
+      <c r="B15">
+        <v>215625</v>
+      </c>
+      <c r="C15">
+        <v>215341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1984</v>
+      </c>
+      <c r="B16">
+        <v>307541</v>
+      </c>
+      <c r="C16">
+        <v>306974</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1985</v>
+      </c>
+      <c r="B17">
+        <v>286900</v>
+      </c>
+      <c r="C17">
+        <v>286907</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1986</v>
+      </c>
+      <c r="B18">
+        <v>86910</v>
+      </c>
+      <c r="C18">
+        <v>86902.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1987</v>
+      </c>
+      <c r="B19">
+        <v>68070</v>
+      </c>
+      <c r="C19">
+        <v>68061.600000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1988</v>
+      </c>
+      <c r="B20">
+        <v>63391</v>
+      </c>
+      <c r="C20">
+        <v>63383.199999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1989</v>
+      </c>
+      <c r="B21">
+        <v>75585</v>
+      </c>
+      <c r="C21">
+        <v>75571.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B22">
+        <v>88269</v>
+      </c>
+      <c r="C22">
+        <v>88268.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1991</v>
+      </c>
+      <c r="B23">
+        <v>100488</v>
+      </c>
+      <c r="C23">
+        <v>100418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1992</v>
+      </c>
+      <c r="B24">
+        <v>90858</v>
+      </c>
+      <c r="C24">
+        <v>90830.399999999994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1993</v>
+      </c>
+      <c r="B25">
+        <v>108909</v>
+      </c>
+      <c r="C25">
+        <v>108571</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1994</v>
+      </c>
+      <c r="B26">
+        <v>107335</v>
+      </c>
+      <c r="C26">
+        <v>106566</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B27">
+        <v>72618</v>
+      </c>
+      <c r="C27">
+        <v>72225.399999999994</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>1996</v>
+      </c>
+      <c r="B28">
+        <v>51263</v>
+      </c>
+      <c r="C28">
+        <v>51080.3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1997</v>
+      </c>
+      <c r="B29">
+        <v>90130</v>
+      </c>
+      <c r="C29">
+        <v>89705.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1998</v>
+      </c>
+      <c r="B30">
+        <v>125460</v>
+      </c>
+      <c r="C30">
+        <v>125107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>1999</v>
+      </c>
+      <c r="B31">
+        <v>95638</v>
+      </c>
+      <c r="C31">
+        <v>95623.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B32">
+        <v>73080</v>
+      </c>
+      <c r="C32">
+        <v>73277.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>2001</v>
+      </c>
+      <c r="B33">
+        <v>72077</v>
+      </c>
+      <c r="C33">
+        <v>72207.399999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>2002</v>
+      </c>
+      <c r="B34">
+        <v>51933.5</v>
+      </c>
+      <c r="C34">
+        <v>51995.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>2003</v>
+      </c>
+      <c r="B35">
+        <v>50684</v>
+      </c>
+      <c r="C35">
+        <v>50814.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>2004</v>
+      </c>
+      <c r="B36">
+        <v>63844</v>
+      </c>
+      <c r="C36">
+        <v>64045.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B37">
+        <v>80978</v>
+      </c>
+      <c r="C37">
+        <v>81425.600000000006</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>2006</v>
+      </c>
+      <c r="B38">
+        <v>71976</v>
+      </c>
+      <c r="C38">
+        <v>72344.899999999994</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>2007</v>
+      </c>
+      <c r="B39">
+        <v>52714</v>
+      </c>
+      <c r="C39">
+        <v>52771.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>2008</v>
+      </c>
+      <c r="B40">
+        <v>52584</v>
+      </c>
+      <c r="C40">
+        <v>52499.199999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B41">
+        <v>44247</v>
+      </c>
+      <c r="C41">
+        <v>44212.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B42">
+        <v>76744</v>
+      </c>
+      <c r="C42">
+        <v>76704.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>2011</v>
+      </c>
+      <c r="B43">
+        <v>81485</v>
+      </c>
+      <c r="C43">
+        <v>81505.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B44">
+        <v>103970</v>
+      </c>
+      <c r="C44">
+        <v>103967</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B45">
+        <v>96364</v>
+      </c>
+      <c r="C45">
+        <v>96525</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B46">
+        <v>142632</v>
+      </c>
+      <c r="C46">
+        <v>143827</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B47">
+        <v>167553</v>
+      </c>
+      <c r="C47">
+        <v>169044</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B48">
+        <v>177134</v>
+      </c>
+      <c r="C48">
+        <v>176780</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B49">
+        <v>186157</v>
+      </c>
+      <c r="C49">
+        <v>185273</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B50">
+        <v>161492</v>
+      </c>
+      <c r="C50">
+        <v>161168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pollock model matches 2018 SAFE
</commit_message>
<xml_diff>
--- a/GOA/Model runs/GOA_18.5.1/Data/2018_SAFE_pollock_estimates.xlsx
+++ b/GOA/Model runs/GOA_18.5.1/Data/2018_SAFE_pollock_estimates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="885" yWindow="1455" windowWidth="24645" windowHeight="13380" activeTab="2"/>
+    <workbookView xWindow="885" yWindow="1455" windowWidth="24645" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="Biomass" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>2018_Pollock</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>2018_safe_no_tv_non_equil</t>
+  </si>
+  <si>
+    <t>2018_no_bt</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:BE4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -439,7 +442,7 @@
     <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -464,8 +467,11 @@
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1970</v>
       </c>
@@ -484,8 +490,11 @@
       <c r="H2">
         <v>0.53080400000000005</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>0.70521199999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1971</v>
       </c>
@@ -504,8 +513,11 @@
       <c r="H3">
         <v>0.52954900000000005</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>0.65474600000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1972</v>
       </c>
@@ -524,8 +536,11 @@
       <c r="H4">
         <v>0.49674000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>0.61271399999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1973</v>
       </c>
@@ -544,8 +559,11 @@
       <c r="H5">
         <v>0.55906100000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>0.66103299999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1974</v>
       </c>
@@ -564,8 +582,11 @@
       <c r="H6">
         <v>0.64705199999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>0.73390299999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1975</v>
       </c>
@@ -584,8 +605,11 @@
       <c r="H7">
         <v>1.2069000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1.2735000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1976</v>
       </c>
@@ -604,8 +628,11 @@
       <c r="H8">
         <v>1.09771</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1.1556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1977</v>
       </c>
@@ -630,8 +657,11 @@
       <c r="H9">
         <v>0.951179</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1.01109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1978</v>
       </c>
@@ -656,8 +686,11 @@
       <c r="H10">
         <v>1.20916</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1.3930499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1979</v>
       </c>
@@ -682,8 +715,11 @@
       <c r="H11">
         <v>1.5669900000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>2.0217700000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1980</v>
       </c>
@@ -708,8 +744,11 @@
       <c r="H12">
         <v>1.9268099999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>2.7965200000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1981</v>
       </c>
@@ -734,8 +773,11 @@
       <c r="H13">
         <v>2.76606</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>4.4247100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1982</v>
       </c>
@@ -760,8 +802,11 @@
       <c r="H14">
         <v>2.86599</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>4.6870399999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1983</v>
       </c>
@@ -786,8 +831,11 @@
       <c r="H15">
         <v>2.6035200000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>4.3681400000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1984</v>
       </c>
@@ -812,8 +860,11 @@
       <c r="H16">
         <v>2.3143799999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>4.0127100000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1985</v>
       </c>
@@ -838,8 +889,11 @@
       <c r="H17">
         <v>1.86574</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>3.39663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1986</v>
       </c>
@@ -864,8 +918,11 @@
       <c r="H18">
         <v>1.59927</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>3.0330599999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1987</v>
       </c>
@@ -890,8 +947,11 @@
       <c r="H19">
         <v>2.03064</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>3.5238700000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1988</v>
       </c>
@@ -916,8 +976,11 @@
       <c r="H20">
         <v>1.96343</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>3.3096100000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1989</v>
       </c>
@@ -942,8 +1005,11 @@
       <c r="H21">
         <v>1.7534700000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>2.9060000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1990</v>
       </c>
@@ -968,8 +1034,11 @@
       <c r="H22">
         <v>1.60755</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>2.6774399999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1991</v>
       </c>
@@ -994,8 +1063,11 @@
       <c r="H23">
         <v>1.8912599999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>3.0335999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1992</v>
       </c>
@@ -1020,8 +1092,11 @@
       <c r="H24">
         <v>1.95903</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>3.1109200000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1993</v>
       </c>
@@ -1046,8 +1121,11 @@
       <c r="H25">
         <v>1.8431200000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>2.9022299999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1994</v>
       </c>
@@ -1072,8 +1150,11 @@
       <c r="H26">
         <v>1.5658000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>2.4740600000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1995</v>
       </c>
@@ -1098,8 +1179,11 @@
       <c r="H27">
         <v>1.2855000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>2.0365600000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1996</v>
       </c>
@@ -1124,8 +1208,11 @@
       <c r="H28">
         <v>1.08104</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>1.71079</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1997</v>
       </c>
@@ -1150,8 +1237,11 @@
       <c r="H29">
         <v>1.0945</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>1.6952499999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1998</v>
       </c>
@@ -1176,8 +1266,11 @@
       <c r="H30">
         <v>1.0425800000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>1.62778</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1999</v>
       </c>
@@ -1202,8 +1295,11 @@
       <c r="H31">
         <v>0.76509199999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1.2570600000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2000</v>
       </c>
@@ -1228,8 +1324,11 @@
       <c r="H32">
         <v>0.66554199999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>1.14516</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2001</v>
       </c>
@@ -1254,8 +1353,11 @@
       <c r="H33">
         <v>0.62135200000000002</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>1.10701</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2002</v>
       </c>
@@ -1280,8 +1382,11 @@
       <c r="H34">
         <v>0.78111699999999995</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>1.38076</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2003</v>
       </c>
@@ -1306,8 +1411,11 @@
       <c r="H35">
         <v>0.98411599999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>1.6688700000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2004</v>
       </c>
@@ -1332,8 +1440,11 @@
       <c r="H36">
         <v>0.81271300000000002</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>1.4131100000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2005</v>
       </c>
@@ -1358,8 +1469,11 @@
       <c r="H37">
         <v>0.67467999999999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>1.19634</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2006</v>
       </c>
@@ -1384,8 +1498,11 @@
       <c r="H38">
         <v>0.56713899999999995</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>1.0517399999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2007</v>
       </c>
@@ -1410,8 +1527,11 @@
       <c r="H39">
         <v>0.53073599999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>0.98543599999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2008</v>
       </c>
@@ -1436,8 +1556,11 @@
       <c r="H40">
         <v>0.77100299999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>1.2663</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2009</v>
       </c>
@@ -1462,8 +1585,11 @@
       <c r="H41">
         <v>1.13452</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>1.68299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2010</v>
       </c>
@@ -1488,8 +1614,11 @@
       <c r="H42">
         <v>1.3858999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>1.92506</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2011</v>
       </c>
@@ -1514,8 +1643,11 @@
       <c r="H43">
         <v>1.3409899999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>1.82003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2012</v>
       </c>
@@ -1540,8 +1672,11 @@
       <c r="H44">
         <v>1.26318</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>1.6891</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2013</v>
       </c>
@@ -1566,8 +1701,11 @@
       <c r="H45">
         <v>1.3071699999999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>1.7353700000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2014</v>
       </c>
@@ -1592,8 +1730,11 @@
       <c r="H46">
         <v>1.0393699999999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>1.38534</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2015</v>
       </c>
@@ -1618,8 +1759,11 @@
       <c r="H47">
         <v>2.2794699999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>3.3017500000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2016</v>
       </c>
@@ -1644,8 +1788,11 @@
       <c r="H48">
         <v>2.2342200000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>3.2779799999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2017</v>
       </c>
@@ -1670,8 +1817,11 @@
       <c r="H49">
         <v>1.61355</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>2.4555699999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2018</v>
       </c>
@@ -1692,6 +1842,9 @@
       </c>
       <c r="H50">
         <v>1.13608</v>
+      </c>
+      <c r="I50">
+        <v>1.8391200000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1701,10 +1854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1712,7 +1865,7 @@
     <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1737,8 +1890,11 @@
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1970</v>
       </c>
@@ -1758,7 +1914,7 @@
         <v>0.13783400000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1971</v>
       </c>
@@ -1778,7 +1934,7 @@
         <v>0.12767899999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1972</v>
       </c>
@@ -1798,7 +1954,7 @@
         <v>0.11670800000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1973</v>
       </c>
@@ -1818,7 +1974,7 @@
         <v>0.100342</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1974</v>
       </c>
@@ -1838,7 +1994,7 @@
         <v>9.3580499999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1975</v>
       </c>
@@ -1858,7 +2014,7 @@
         <v>0.10065499999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1976</v>
       </c>
@@ -1878,7 +2034,7 @@
         <v>0.14930499999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1977</v>
       </c>
@@ -1904,7 +2060,7 @@
         <v>0.17261499999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1978</v>
       </c>
@@ -1930,7 +2086,7 @@
         <v>0.16469600000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1979</v>
       </c>
@@ -1956,7 +2112,7 @@
         <v>0.17421800000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1980</v>
       </c>
@@ -1982,7 +2138,7 @@
         <v>0.22292400000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1981</v>
       </c>
@@ -2008,7 +2164,7 @@
         <v>0.22394</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1982</v>
       </c>
@@ -2034,7 +2190,7 @@
         <v>0.340615</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1983</v>
       </c>
@@ -2060,7 +2216,7 @@
         <v>0.44499499999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1984</v>
       </c>
@@ -2974,10 +3130,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2985,7 +3141,7 @@
     <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3010,8 +3166,11 @@
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1970</v>
       </c>
@@ -3031,7 +3190,7 @@
         <v>1.39063</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1971</v>
       </c>
@@ -3051,7 +3210,7 @@
         <v>3.52562</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1972</v>
       </c>
@@ -3071,7 +3230,7 @@
         <v>4.2795100000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1973</v>
       </c>
@@ -3091,7 +3250,7 @@
         <v>13.167</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1974</v>
       </c>
@@ -3111,7 +3270,7 @@
         <v>2.7866900000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1975</v>
       </c>
@@ -3131,7 +3290,7 @@
         <v>2.7593899999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1976</v>
       </c>
@@ -3151,7 +3310,7 @@
         <v>10.011699999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1977</v>
       </c>
@@ -3177,7 +3336,7 @@
         <v>12.1051</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1978</v>
       </c>
@@ -3203,7 +3362,7 @@
         <v>13.15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1979</v>
       </c>
@@ -3229,7 +3388,7 @@
         <v>22.679500000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1980</v>
       </c>
@@ -3255,7 +3414,7 @@
         <v>12.440300000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1981</v>
       </c>
@@ -3281,7 +3440,7 @@
         <v>7.1817399999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1982</v>
       </c>
@@ -3307,7 +3466,7 @@
         <v>7.1661900000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>1983</v>
       </c>
@@ -3333,7 +3492,7 @@
         <v>4.9868800000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1984</v>
       </c>

</xml_diff>